<commit_message>
Thu Nov 28 03:58:49 PM EST 2024
</commit_message>
<xml_diff>
--- a/parallel/988-v_energies.xlsx
+++ b/parallel/988-v_energies.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6896613841</v>
+        <v>-0.6896612906</v>
       </c>
     </row>
     <row r="3">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-7025.08916198</v>
+        <v>-7025.08916189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>